<commit_message>
Update test matrix for Windows 11 22H2
</commit_message>
<xml_diff>
--- a/test-matrix.xlsx
+++ b/test-matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>This chart updated:</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>VS2017 15.9.50</t>
+  </si>
+  <si>
+    <t>Windows 11</t>
+  </si>
+  <si>
+    <t>Pro 22H2</t>
+  </si>
+  <si>
+    <t>PowerShell 7.1.3</t>
+  </si>
+  <si>
+    <t>VS2019 16.11.21</t>
+  </si>
+  <si>
+    <t>VS2017 15.9.51</t>
+  </si>
+  <si>
+    <t>VS2022 17.4.1</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H15"/>
+  <dimension ref="A2:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -488,7 +506,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="3">
         <f ca="1">TODAY()</f>
-        <v>44824</v>
+        <v>44889</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -554,10 +572,10 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>2</v>
@@ -566,21 +584,21 @@
         <v>12</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G13" s="8">
-        <v>44824</v>
+        <v>44888</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
@@ -592,21 +610,21 @@
         <v>12</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G14" s="8">
-        <v>44824</v>
+        <v>44888</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>18</v>
@@ -618,15 +636,93 @@
         <v>12</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="8">
+        <v>44888</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="8">
         <v>44824</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8">
+        <v>44824</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="8">
+        <v>44824</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>